<commit_message>
BSTATS-152: Scoresheet - way to enter visiting players
</commit_message>
<xml_diff>
--- a/teams_CIN_1961-roster_appearances.xlsx
+++ b/teams_CIN_1961-roster_appearances.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -1165,9 +1165,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AB40"/>
+  <dimension ref="A2:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4115,86 +4117,6 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40" t="s">
-        <v>3</v>
-      </c>
-      <c r="F40" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" t="s">
-        <v>6</v>
-      </c>
-      <c r="I40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J40" t="s">
-        <v>8</v>
-      </c>
-      <c r="K40" t="s">
-        <v>9</v>
-      </c>
-      <c r="L40" t="s">
-        <v>10</v>
-      </c>
-      <c r="M40" t="s">
-        <v>11</v>
-      </c>
-      <c r="N40" t="s">
-        <v>12</v>
-      </c>
-      <c r="O40" t="s">
-        <v>13</v>
-      </c>
-      <c r="P40" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>15</v>
-      </c>
-      <c r="R40" t="s">
-        <v>16</v>
-      </c>
-      <c r="S40" t="s">
-        <v>17</v>
-      </c>
-      <c r="T40" t="s">
-        <v>18</v>
-      </c>
-      <c r="U40" t="s">
-        <v>19</v>
-      </c>
-      <c r="V40" t="s">
-        <v>20</v>
-      </c>
-      <c r="W40" t="s">
-        <v>21</v>
-      </c>
-      <c r="X40" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>